<commit_message>
edit final doc part 1
</commit_message>
<xml_diff>
--- a/PhanTich - Thiet Ke - CarPoly/BangPhanCongCongViec.xlsx
+++ b/PhanTich - Thiet Ke - CarPoly/BangPhanCongCongViec.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai Lieu\KyThuatPhanMem\CarPoly\PhanTich - Thiet Ke - CarPoly\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>BẢNG PHÂN CÔNG</t>
   </si>
@@ -132,12 +127,18 @@
   </si>
   <si>
     <t>SV4</t>
+  </si>
+  <si>
+    <t>PS09095</t>
+  </si>
+  <si>
+    <t>PS09117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,16 +257,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -740,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,23 +752,23 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -775,7 +776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -783,52 +784,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -839,7 +840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -850,25 +851,29 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -894,7 +899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -904,10 +909,10 @@
       <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="9">
         <v>43839</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="9">
         <v>43841</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -917,7 +922,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -927,10 +932,10 @@
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="9">
         <v>43843</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="9">
         <v>43844</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -940,7 +945,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -950,10 +955,10 @@
       <c r="C18" s="1">
         <v>5</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="9">
         <v>43850</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="9">
         <v>43854</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -963,7 +968,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -973,10 +978,10 @@
       <c r="C19" s="1">
         <v>4</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="9">
         <v>43878</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="10">
         <v>43881</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -986,7 +991,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -996,10 +1001,10 @@
       <c r="C20" s="1">
         <v>3</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="9">
         <v>43882</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="9">
         <v>43884</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1009,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1019,10 +1024,10 @@
       <c r="C21" s="1">
         <v>3</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="9">
         <v>43874</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="9">
         <v>43876</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1032,7 +1037,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -1042,20 +1047,20 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="9">
         <v>43889</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="9">
         <v>43889</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:G6"/>

</xml_diff>

<commit_message>
Update Bang Phan Cong (Excel)
</commit_message>
<xml_diff>
--- a/PhanTich - Thiet Ke - CarPoly/BangPhanCongCongViec.xlsx
+++ b/PhanTich - Thiet Ke - CarPoly/BangPhanCongCongViec.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tai Lieu\KyThuatPhanMem\CarPoly\PhanTich - Thiet Ke - CarPoly\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,7 +143,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -741,7 +746,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,24 +756,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>31</v>
       </c>
@@ -776,7 +781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
@@ -784,7 +789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -794,7 +799,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -802,7 +807,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -810,7 +815,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="12" t="s">
         <v>2</v>
@@ -821,15 +826,15 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
@@ -840,7 +845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -851,7 +856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -862,7 +867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
@@ -873,7 +878,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -899,7 +904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -919,10 +924,10 @@
         <v>27</v>
       </c>
       <c r="H16" s="5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -942,10 +947,10 @@
         <v>27</v>
       </c>
       <c r="H17" s="5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>3</v>
       </c>
@@ -965,10 +970,10 @@
         <v>34</v>
       </c>
       <c r="H18" s="5">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>4</v>
       </c>
@@ -988,10 +993,10 @@
         <v>27</v>
       </c>
       <c r="H19" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>5</v>
       </c>
@@ -1014,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -1034,10 +1039,10 @@
         <v>29</v>
       </c>
       <c r="H21" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>7</v>
       </c>
@@ -1056,11 +1061,14 @@
       <c r="G22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:G6"/>

</xml_diff>